<commit_message>
Multi threading in for different test configs
</commit_message>
<xml_diff>
--- a/main_sheet.xlsx
+++ b/main_sheet.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>test_path</t>
   </si>
@@ -26,6 +26,9 @@
     <t>url</t>
   </si>
   <si>
+    <t>name</t>
+  </si>
+  <si>
     <t>test1/test_sheet.xlsx</t>
   </si>
   <si>
@@ -33,6 +36,12 @@
   </si>
   <si>
     <t>http://localhost:9001</t>
+  </si>
+  <si>
+    <t>test_1</t>
+  </si>
+  <si>
+    <t>Test_2</t>
   </si>
 </sst>
 </file>
@@ -140,10 +149,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -164,21 +173,42 @@
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="B3" s="0" t="s">
         <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="http://localhost:9001"/>
+    <hyperlink ref="C3" r:id="rId2" display="http://localhost:9001"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>